<commit_message>
clean up, and calculate the overlap between HISAT2 and EAGLERC mapping results.
</commit_message>
<xml_diff>
--- a/files/SI_Data_4__CS_PERNASeq.xlsx
+++ b/files/SI_Data_4__CS_PERNASeq.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsun/Google Drive/projects/HuoberBrezel/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F83502D-9694-D646-AEEB-0CEECC821B02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A94D2B1-95BF-9742-99B3-091329B2C82B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="9960" activeTab="4" xr2:uid="{0A1B866E-BAB2-5B48-9BA1-056163FF4A88}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25440" windowHeight="9960" activeTab="1" xr2:uid="{0A1B866E-BAB2-5B48-9BA1-056163FF4A88}"/>
   </bookViews>
   <sheets>
     <sheet name="Trimmomatic" sheetId="6" r:id="rId1"/>
     <sheet name="HISAT2" sheetId="5" r:id="rId2"/>
     <sheet name="STAR" sheetId="7" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="8" r:id="rId4"/>
-    <sheet name="EAGLE-RC" sheetId="4" r:id="rId5"/>
+    <sheet name="EAGLE-RC" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="68">
   <si>
     <t>library name</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>EAGLE-RC step</t>
+  </si>
+  <si>
+    <t>% effective reads</t>
   </si>
 </sst>
 </file>
@@ -950,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF108285-BE0D-0046-88C0-1ED8933A3288}">
   <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2054,8 +2057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C48FE8-9208-1D4A-9BAC-FDFBEF8F0685}">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2624,743 +2627,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FBA10C5-DEDA-5944-A06B-7BB4E891A333}">
-  <dimension ref="A1:Q78"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3:Q8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" t="s">
-        <v>59</v>
-      </c>
-      <c r="K2" t="s">
-        <v>60</v>
-      </c>
-      <c r="N2" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>27407286</v>
-      </c>
-      <c r="F3">
-        <v>27407286</v>
-      </c>
-      <c r="G3">
-        <v>199774</v>
-      </c>
-      <c r="H3" s="4">
-        <f>F3/2+G3</f>
-        <v>13903417</v>
-      </c>
-      <c r="I3">
-        <v>8564432</v>
-      </c>
-      <c r="J3">
-        <v>64650</v>
-      </c>
-      <c r="K3" s="4">
-        <f>I3/2+J3</f>
-        <v>4346866</v>
-      </c>
-      <c r="L3">
-        <v>9347120</v>
-      </c>
-      <c r="M3">
-        <v>67802</v>
-      </c>
-      <c r="N3" s="4">
-        <f>L3/2+M3</f>
-        <v>4741362</v>
-      </c>
-      <c r="O3">
-        <v>9153656</v>
-      </c>
-      <c r="P3">
-        <v>64603</v>
-      </c>
-      <c r="Q3" s="4">
-        <f>O3/2+P3</f>
-        <v>4641431</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>199774</v>
-      </c>
-      <c r="F4">
-        <v>24629078</v>
-      </c>
-      <c r="G4">
-        <v>202433</v>
-      </c>
-      <c r="H4" s="4">
-        <f t="shared" ref="H4:H8" si="0">F4/2+G4</f>
-        <v>12516972</v>
-      </c>
-      <c r="I4">
-        <v>7792682</v>
-      </c>
-      <c r="J4">
-        <v>65545</v>
-      </c>
-      <c r="K4" s="4">
-        <f t="shared" ref="K4:K8" si="1">I4/2+J4</f>
-        <v>3961886</v>
-      </c>
-      <c r="L4">
-        <v>8451068</v>
-      </c>
-      <c r="M4">
-        <v>69589</v>
-      </c>
-      <c r="N4" s="4">
-        <f t="shared" ref="N4:N8" si="2">L4/2+M4</f>
-        <v>4295123</v>
-      </c>
-      <c r="O4">
-        <v>8111402</v>
-      </c>
-      <c r="P4">
-        <v>64821</v>
-      </c>
-      <c r="Q4" s="4">
-        <f t="shared" ref="Q4:Q8" si="3">O4/2+P4</f>
-        <v>4120522</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5">
-        <v>18020724</v>
-      </c>
-      <c r="G5">
-        <v>144117</v>
-      </c>
-      <c r="H5" s="4">
-        <f t="shared" si="0"/>
-        <v>9154479</v>
-      </c>
-      <c r="I5">
-        <v>5768460</v>
-      </c>
-      <c r="J5">
-        <v>47029</v>
-      </c>
-      <c r="K5" s="4">
-        <f t="shared" si="1"/>
-        <v>2931259</v>
-      </c>
-      <c r="L5">
-        <v>6148394</v>
-      </c>
-      <c r="M5">
-        <v>49432</v>
-      </c>
-      <c r="N5" s="4">
-        <f t="shared" si="2"/>
-        <v>3123629</v>
-      </c>
-      <c r="O5">
-        <v>5909548</v>
-      </c>
-      <c r="P5">
-        <v>46003</v>
-      </c>
-      <c r="Q5" s="4">
-        <f t="shared" si="3"/>
-        <v>3000777</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>8564432</v>
-      </c>
-      <c r="F6">
-        <v>25227486</v>
-      </c>
-      <c r="G6">
-        <v>160715</v>
-      </c>
-      <c r="H6" s="4">
-        <f t="shared" si="0"/>
-        <v>12774458</v>
-      </c>
-      <c r="I6">
-        <v>7990190</v>
-      </c>
-      <c r="J6">
-        <v>52119</v>
-      </c>
-      <c r="K6" s="4">
-        <f t="shared" si="1"/>
-        <v>4047214</v>
-      </c>
-      <c r="L6">
-        <v>8682364</v>
-      </c>
-      <c r="M6">
-        <v>54954</v>
-      </c>
-      <c r="N6" s="4">
-        <f t="shared" si="2"/>
-        <v>4396136</v>
-      </c>
-      <c r="O6">
-        <v>8270912</v>
-      </c>
-      <c r="P6">
-        <v>51751</v>
-      </c>
-      <c r="Q6" s="4">
-        <f t="shared" si="3"/>
-        <v>4187207</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>64650</v>
-      </c>
-      <c r="F7">
-        <v>32981640</v>
-      </c>
-      <c r="G7">
-        <v>267937</v>
-      </c>
-      <c r="H7" s="4">
-        <f t="shared" si="0"/>
-        <v>16758757</v>
-      </c>
-      <c r="I7">
-        <v>10567204</v>
-      </c>
-      <c r="J7">
-        <v>87061</v>
-      </c>
-      <c r="K7" s="4">
-        <f t="shared" si="1"/>
-        <v>5370663</v>
-      </c>
-      <c r="L7">
-        <v>11314588</v>
-      </c>
-      <c r="M7">
-        <v>91753</v>
-      </c>
-      <c r="N7" s="4">
-        <f t="shared" si="2"/>
-        <v>5749047</v>
-      </c>
-      <c r="O7">
-        <v>10759780</v>
-      </c>
-      <c r="P7">
-        <v>86195</v>
-      </c>
-      <c r="Q7" s="4">
-        <f t="shared" si="3"/>
-        <v>5466085</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8">
-        <v>32299428</v>
-      </c>
-      <c r="G8">
-        <v>202697</v>
-      </c>
-      <c r="H8" s="4">
-        <f t="shared" si="0"/>
-        <v>16352411</v>
-      </c>
-      <c r="I8">
-        <v>10216736</v>
-      </c>
-      <c r="J8">
-        <v>65707</v>
-      </c>
-      <c r="K8" s="4">
-        <f t="shared" si="1"/>
-        <v>5174075</v>
-      </c>
-      <c r="L8">
-        <v>10960450</v>
-      </c>
-      <c r="M8">
-        <v>68603</v>
-      </c>
-      <c r="N8" s="4">
-        <f t="shared" si="2"/>
-        <v>5548828</v>
-      </c>
-      <c r="O8">
-        <v>10758284</v>
-      </c>
-      <c r="P8">
-        <v>65974</v>
-      </c>
-      <c r="Q8" s="4">
-        <f t="shared" si="3"/>
-        <v>5445116</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>9347120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>67802</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>9153656</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>64603</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>24629078</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>202433</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>7792682</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>65545</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>8451068</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>69589</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>8111402</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>64821</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>18020724</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>144117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>5768460</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>47029</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>6148394</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>49432</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>5909548</v>
-      </c>
-      <c r="F38">
-        <v>25227486</v>
-      </c>
-      <c r="G38">
-        <v>160715</v>
-      </c>
-      <c r="I38">
-        <v>7990190</v>
-      </c>
-      <c r="J38">
-        <v>52119</v>
-      </c>
-      <c r="L38">
-        <v>8682364</v>
-      </c>
-      <c r="M38">
-        <v>54954</v>
-      </c>
-      <c r="O38">
-        <v>8270912</v>
-      </c>
-      <c r="P38">
-        <v>51751</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>46003</v>
-      </c>
-      <c r="F39">
-        <v>32981640</v>
-      </c>
-      <c r="G39">
-        <v>267937</v>
-      </c>
-      <c r="I39">
-        <v>10567204</v>
-      </c>
-      <c r="J39">
-        <v>87061</v>
-      </c>
-      <c r="L39">
-        <v>11314588</v>
-      </c>
-      <c r="M39">
-        <v>91753</v>
-      </c>
-      <c r="O39">
-        <v>10759780</v>
-      </c>
-      <c r="P39">
-        <v>86195</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F40">
-        <v>32299428</v>
-      </c>
-      <c r="G40">
-        <v>202697</v>
-      </c>
-      <c r="I40">
-        <v>10216736</v>
-      </c>
-      <c r="J40">
-        <v>65707</v>
-      </c>
-      <c r="L40">
-        <v>10960450</v>
-      </c>
-      <c r="M40">
-        <v>68603</v>
-      </c>
-      <c r="O40">
-        <v>10758284</v>
-      </c>
-      <c r="P40">
-        <v>65974</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>25227486</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>160715</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>7990190</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>52119</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>8682364</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>54954</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>8270912</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>51751</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>32981640</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>267937</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>10567204</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>87061</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>11314588</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>91753</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>10759780</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>86195</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>32299428</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>202697</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>10216736</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>65707</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>10960450</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>68603</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>10758284</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>65974</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{637DE6A1-0D97-9640-86A6-1F46B9A691B7}">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:G13"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3431,7 +2702,7 @@
         <v>35</v>
       </c>
       <c r="T1" s="31" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -4239,4 +3510,736 @@
     <ignoredError sqref="H17:H19 H14:H16" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FBA10C5-DEDA-5944-A06B-7BB4E891A333}">
+  <dimension ref="A1:Q78"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3:Q8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>27407286</v>
+      </c>
+      <c r="F3">
+        <v>27407286</v>
+      </c>
+      <c r="G3">
+        <v>199774</v>
+      </c>
+      <c r="H3" s="4">
+        <f>F3/2+G3</f>
+        <v>13903417</v>
+      </c>
+      <c r="I3">
+        <v>8564432</v>
+      </c>
+      <c r="J3">
+        <v>64650</v>
+      </c>
+      <c r="K3" s="4">
+        <f>I3/2+J3</f>
+        <v>4346866</v>
+      </c>
+      <c r="L3">
+        <v>9347120</v>
+      </c>
+      <c r="M3">
+        <v>67802</v>
+      </c>
+      <c r="N3" s="4">
+        <f>L3/2+M3</f>
+        <v>4741362</v>
+      </c>
+      <c r="O3">
+        <v>9153656</v>
+      </c>
+      <c r="P3">
+        <v>64603</v>
+      </c>
+      <c r="Q3" s="4">
+        <f>O3/2+P3</f>
+        <v>4641431</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>199774</v>
+      </c>
+      <c r="F4">
+        <v>24629078</v>
+      </c>
+      <c r="G4">
+        <v>202433</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" ref="H4:H8" si="0">F4/2+G4</f>
+        <v>12516972</v>
+      </c>
+      <c r="I4">
+        <v>7792682</v>
+      </c>
+      <c r="J4">
+        <v>65545</v>
+      </c>
+      <c r="K4" s="4">
+        <f t="shared" ref="K4:K8" si="1">I4/2+J4</f>
+        <v>3961886</v>
+      </c>
+      <c r="L4">
+        <v>8451068</v>
+      </c>
+      <c r="M4">
+        <v>69589</v>
+      </c>
+      <c r="N4" s="4">
+        <f t="shared" ref="N4:N8" si="2">L4/2+M4</f>
+        <v>4295123</v>
+      </c>
+      <c r="O4">
+        <v>8111402</v>
+      </c>
+      <c r="P4">
+        <v>64821</v>
+      </c>
+      <c r="Q4" s="4">
+        <f t="shared" ref="Q4:Q8" si="3">O4/2+P4</f>
+        <v>4120522</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5">
+        <v>18020724</v>
+      </c>
+      <c r="G5">
+        <v>144117</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" si="0"/>
+        <v>9154479</v>
+      </c>
+      <c r="I5">
+        <v>5768460</v>
+      </c>
+      <c r="J5">
+        <v>47029</v>
+      </c>
+      <c r="K5" s="4">
+        <f t="shared" si="1"/>
+        <v>2931259</v>
+      </c>
+      <c r="L5">
+        <v>6148394</v>
+      </c>
+      <c r="M5">
+        <v>49432</v>
+      </c>
+      <c r="N5" s="4">
+        <f t="shared" si="2"/>
+        <v>3123629</v>
+      </c>
+      <c r="O5">
+        <v>5909548</v>
+      </c>
+      <c r="P5">
+        <v>46003</v>
+      </c>
+      <c r="Q5" s="4">
+        <f t="shared" si="3"/>
+        <v>3000777</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>8564432</v>
+      </c>
+      <c r="F6">
+        <v>25227486</v>
+      </c>
+      <c r="G6">
+        <v>160715</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" si="0"/>
+        <v>12774458</v>
+      </c>
+      <c r="I6">
+        <v>7990190</v>
+      </c>
+      <c r="J6">
+        <v>52119</v>
+      </c>
+      <c r="K6" s="4">
+        <f t="shared" si="1"/>
+        <v>4047214</v>
+      </c>
+      <c r="L6">
+        <v>8682364</v>
+      </c>
+      <c r="M6">
+        <v>54954</v>
+      </c>
+      <c r="N6" s="4">
+        <f t="shared" si="2"/>
+        <v>4396136</v>
+      </c>
+      <c r="O6">
+        <v>8270912</v>
+      </c>
+      <c r="P6">
+        <v>51751</v>
+      </c>
+      <c r="Q6" s="4">
+        <f t="shared" si="3"/>
+        <v>4187207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>64650</v>
+      </c>
+      <c r="F7">
+        <v>32981640</v>
+      </c>
+      <c r="G7">
+        <v>267937</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="0"/>
+        <v>16758757</v>
+      </c>
+      <c r="I7">
+        <v>10567204</v>
+      </c>
+      <c r="J7">
+        <v>87061</v>
+      </c>
+      <c r="K7" s="4">
+        <f t="shared" si="1"/>
+        <v>5370663</v>
+      </c>
+      <c r="L7">
+        <v>11314588</v>
+      </c>
+      <c r="M7">
+        <v>91753</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" si="2"/>
+        <v>5749047</v>
+      </c>
+      <c r="O7">
+        <v>10759780</v>
+      </c>
+      <c r="P7">
+        <v>86195</v>
+      </c>
+      <c r="Q7" s="4">
+        <f t="shared" si="3"/>
+        <v>5466085</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8">
+        <v>32299428</v>
+      </c>
+      <c r="G8">
+        <v>202697</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="0"/>
+        <v>16352411</v>
+      </c>
+      <c r="I8">
+        <v>10216736</v>
+      </c>
+      <c r="J8">
+        <v>65707</v>
+      </c>
+      <c r="K8" s="4">
+        <f t="shared" si="1"/>
+        <v>5174075</v>
+      </c>
+      <c r="L8">
+        <v>10960450</v>
+      </c>
+      <c r="M8">
+        <v>68603</v>
+      </c>
+      <c r="N8" s="4">
+        <f t="shared" si="2"/>
+        <v>5548828</v>
+      </c>
+      <c r="O8">
+        <v>10758284</v>
+      </c>
+      <c r="P8">
+        <v>65974</v>
+      </c>
+      <c r="Q8" s="4">
+        <f t="shared" si="3"/>
+        <v>5445116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>9347120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>67802</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>9153656</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>64603</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>24629078</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>202433</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>7792682</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>65545</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>8451068</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>69589</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>8111402</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>64821</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>18020724</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>144117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>5768460</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>47029</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>6148394</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>49432</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>5909548</v>
+      </c>
+      <c r="F38">
+        <v>25227486</v>
+      </c>
+      <c r="G38">
+        <v>160715</v>
+      </c>
+      <c r="I38">
+        <v>7990190</v>
+      </c>
+      <c r="J38">
+        <v>52119</v>
+      </c>
+      <c r="L38">
+        <v>8682364</v>
+      </c>
+      <c r="M38">
+        <v>54954</v>
+      </c>
+      <c r="O38">
+        <v>8270912</v>
+      </c>
+      <c r="P38">
+        <v>51751</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>46003</v>
+      </c>
+      <c r="F39">
+        <v>32981640</v>
+      </c>
+      <c r="G39">
+        <v>267937</v>
+      </c>
+      <c r="I39">
+        <v>10567204</v>
+      </c>
+      <c r="J39">
+        <v>87061</v>
+      </c>
+      <c r="L39">
+        <v>11314588</v>
+      </c>
+      <c r="M39">
+        <v>91753</v>
+      </c>
+      <c r="O39">
+        <v>10759780</v>
+      </c>
+      <c r="P39">
+        <v>86195</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>56</v>
+      </c>
+      <c r="F40">
+        <v>32299428</v>
+      </c>
+      <c r="G40">
+        <v>202697</v>
+      </c>
+      <c r="I40">
+        <v>10216736</v>
+      </c>
+      <c r="J40">
+        <v>65707</v>
+      </c>
+      <c r="L40">
+        <v>10960450</v>
+      </c>
+      <c r="M40">
+        <v>68603</v>
+      </c>
+      <c r="O40">
+        <v>10758284</v>
+      </c>
+      <c r="P40">
+        <v>65974</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>25227486</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>160715</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>7990190</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>52119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>8682364</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>54954</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>8270912</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51751</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>32981640</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>267937</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>10567204</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>87061</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>11314588</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>91753</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>10759780</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>86195</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>32299428</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>202697</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>10216736</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>65707</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>10960450</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>68603</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>10758284</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>65974</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>